<commit_message>
Fixed changes and made changes
</commit_message>
<xml_diff>
--- a/sample-input-data/YUVA.xlsx
+++ b/sample-input-data/YUVA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anish\Documents\FullStack\exam-seating\sample-input-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FDEB20-E51B-4658-934A-4F92B3C270A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A2F9834-F8D5-4776-B871-583AFF4244AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7344" yWindow="3684" windowWidth="16284" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="294">
   <si>
     <t>section</t>
   </si>
@@ -903,6 +903,12 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>SUPIKSHA P CP</t>
+  </si>
+  <si>
+    <t>SREYA SRI R</t>
   </si>
 </sst>
 </file>
@@ -1233,16 +1239,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S998"/>
+  <dimension ref="A1:S994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.5546875" style="12" customWidth="1"/>
-    <col min="2" max="3" width="14.44140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="28" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" style="12" customWidth="1"/>
   </cols>
@@ -1285,13 +1292,13 @@
       <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="8">
+        <v>921321104001</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
@@ -1316,13 +1323,13 @@
       <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="8">
+        <v>921321104002</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
@@ -1347,13 +1354,13 @@
       <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="8">
+        <v>921321104003</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="1"/>
@@ -1378,13 +1385,13 @@
       <c r="B5" s="5">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="C5" s="8">
+        <v>921321104004</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="1"/>
@@ -1409,13 +1416,13 @@
       <c r="B6" s="5">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="8">
+        <v>921321104005</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F6" s="1"/>
@@ -1441,10 +1448,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="8">
-        <v>921321104001</v>
+        <v>921321104006</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>1</v>
@@ -1472,10 +1479,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="8">
-        <v>921321104002</v>
+        <v>921321104007</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>1</v>
@@ -1503,10 +1510,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="8">
-        <v>921321104003</v>
+        <v>921321104008</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>1</v>
@@ -1534,10 +1541,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="8">
-        <v>921321104004</v>
+        <v>921321104009</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>1</v>
@@ -1565,10 +1572,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="8">
-        <v>921321104005</v>
+        <v>921321104010</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>1</v>
@@ -1596,10 +1603,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="8">
-        <v>921321104006</v>
+        <v>921321104011</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>1</v>
@@ -1627,10 +1634,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="8">
-        <v>921321104007</v>
+        <v>921321104012</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>1</v>
@@ -1658,10 +1665,10 @@
         <v>13</v>
       </c>
       <c r="C14" s="8">
-        <v>921321104008</v>
+        <v>921321104013</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>1</v>
@@ -1689,10 +1696,10 @@
         <v>14</v>
       </c>
       <c r="C15" s="8">
-        <v>921321104009</v>
+        <v>921321104014</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>1</v>
@@ -1712,7 +1719,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1720,10 +1727,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="8">
-        <v>921321104010</v>
+        <v>921321104015</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>1</v>
@@ -1743,7 +1750,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1751,10 +1758,10 @@
         <v>16</v>
       </c>
       <c r="C17" s="8">
-        <v>921321104011</v>
+        <v>921321104016</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>1</v>
@@ -1774,7 +1781,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1782,10 +1789,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="8">
-        <v>921321104012</v>
+        <v>921321104017</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>1</v>
@@ -1805,7 +1812,7 @@
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1813,10 +1820,10 @@
         <v>18</v>
       </c>
       <c r="C19" s="8">
-        <v>921321104013</v>
+        <v>921321104018</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>1</v>
@@ -1836,7 +1843,7 @@
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1844,10 +1851,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="8">
-        <v>921321104014</v>
+        <v>921321104019</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>1</v>
@@ -1875,10 +1882,10 @@
         <v>20</v>
       </c>
       <c r="C21" s="8">
-        <v>921321104015</v>
+        <v>921321104020</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>1</v>
@@ -1906,10 +1913,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="8">
-        <v>921321104016</v>
+        <v>921321104021</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>1</v>
@@ -1937,10 +1944,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="8">
-        <v>921321104017</v>
+        <v>921321104022</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>1</v>
@@ -1968,10 +1975,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="8">
-        <v>921321104018</v>
+        <v>921321104023</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>1</v>
@@ -1999,10 +2006,10 @@
         <v>24</v>
       </c>
       <c r="C25" s="8">
-        <v>921321104019</v>
+        <v>921321104024</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>1</v>
@@ -2030,10 +2037,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="8">
-        <v>921321104020</v>
+        <v>921321104025</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>1</v>
@@ -2061,10 +2068,10 @@
         <v>26</v>
       </c>
       <c r="C27" s="8">
-        <v>921321104021</v>
+        <v>921321104026</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>1</v>
@@ -2092,10 +2099,10 @@
         <v>27</v>
       </c>
       <c r="C28" s="8">
-        <v>921321104022</v>
+        <v>921321104027</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>1</v>
@@ -2123,10 +2130,10 @@
         <v>28</v>
       </c>
       <c r="C29" s="8">
-        <v>921321104023</v>
+        <v>921321104028</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>1</v>
@@ -2154,10 +2161,10 @@
         <v>29</v>
       </c>
       <c r="C30" s="8">
-        <v>921321104024</v>
+        <v>921321104029</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>1</v>
@@ -2185,10 +2192,10 @@
         <v>30</v>
       </c>
       <c r="C31" s="8">
-        <v>921321104025</v>
+        <v>921321104030</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>1</v>
@@ -2216,10 +2223,10 @@
         <v>31</v>
       </c>
       <c r="C32" s="8">
-        <v>921321104026</v>
+        <v>921321104031</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>1</v>
@@ -2247,10 +2254,10 @@
         <v>32</v>
       </c>
       <c r="C33" s="8">
-        <v>921321104027</v>
+        <v>921321104032</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>1</v>
@@ -2278,10 +2285,10 @@
         <v>33</v>
       </c>
       <c r="C34" s="8">
-        <v>921321104028</v>
+        <v>921321104033</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>1</v>
@@ -2309,10 +2316,10 @@
         <v>34</v>
       </c>
       <c r="C35" s="8">
-        <v>921321104029</v>
+        <v>921321104034</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>1</v>
@@ -2340,10 +2347,10 @@
         <v>35</v>
       </c>
       <c r="C36" s="8">
-        <v>921321104030</v>
+        <v>921321104035</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>1</v>
@@ -2371,10 +2378,10 @@
         <v>36</v>
       </c>
       <c r="C37" s="8">
-        <v>921321104031</v>
+        <v>921321104036</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>1</v>
@@ -2402,10 +2409,10 @@
         <v>37</v>
       </c>
       <c r="C38" s="8">
-        <v>921321104032</v>
+        <v>921321104037</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>1</v>
@@ -2433,10 +2440,10 @@
         <v>38</v>
       </c>
       <c r="C39" s="8">
-        <v>921321104033</v>
+        <v>921321104038</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>1</v>
@@ -2464,10 +2471,10 @@
         <v>39</v>
       </c>
       <c r="C40" s="8">
-        <v>921321104034</v>
+        <v>921321104039</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>1</v>
@@ -2495,10 +2502,10 @@
         <v>40</v>
       </c>
       <c r="C41" s="8">
-        <v>921321104035</v>
+        <v>921321104040</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>1</v>
@@ -2526,10 +2533,10 @@
         <v>41</v>
       </c>
       <c r="C42" s="8">
-        <v>921321104036</v>
+        <v>921321104041</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>1</v>
@@ -2557,10 +2564,10 @@
         <v>42</v>
       </c>
       <c r="C43" s="8">
-        <v>921321104037</v>
+        <v>921321104042</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>1</v>
@@ -2588,10 +2595,10 @@
         <v>43</v>
       </c>
       <c r="C44" s="8">
-        <v>921321104038</v>
+        <v>921321104043</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>1</v>
@@ -2619,10 +2626,10 @@
         <v>44</v>
       </c>
       <c r="C45" s="8">
-        <v>921321104039</v>
+        <v>921321104044</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>1</v>
@@ -2650,10 +2657,10 @@
         <v>45</v>
       </c>
       <c r="C46" s="8">
-        <v>921321104040</v>
+        <v>921321104045</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>1</v>
@@ -2681,10 +2688,10 @@
         <v>46</v>
       </c>
       <c r="C47" s="8">
-        <v>921321104041</v>
+        <v>921321104046</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>1</v>
@@ -2712,10 +2719,10 @@
         <v>47</v>
       </c>
       <c r="C48" s="8">
-        <v>921321104042</v>
+        <v>921321104047</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>1</v>
@@ -2743,10 +2750,10 @@
         <v>48</v>
       </c>
       <c r="C49" s="8">
-        <v>921321104043</v>
+        <v>921321104048</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>1</v>
@@ -2774,10 +2781,10 @@
         <v>49</v>
       </c>
       <c r="C50" s="8">
-        <v>921321104044</v>
+        <v>921321104049</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E50" s="7" t="s">
         <v>1</v>
@@ -2805,10 +2812,10 @@
         <v>50</v>
       </c>
       <c r="C51" s="8">
-        <v>921321104045</v>
+        <v>921321104050</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E51" s="7" t="s">
         <v>1</v>
@@ -2836,10 +2843,10 @@
         <v>51</v>
       </c>
       <c r="C52" s="8">
-        <v>921321104046</v>
+        <v>921321104051</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E52" s="7" t="s">
         <v>1</v>
@@ -2867,10 +2874,10 @@
         <v>52</v>
       </c>
       <c r="C53" s="8">
-        <v>921321104047</v>
+        <v>921321104052</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>1</v>
@@ -2898,10 +2905,10 @@
         <v>53</v>
       </c>
       <c r="C54" s="8">
-        <v>921321104048</v>
+        <v>921321104053</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E54" s="7" t="s">
         <v>1</v>
@@ -2929,10 +2936,10 @@
         <v>54</v>
       </c>
       <c r="C55" s="8">
-        <v>921321104049</v>
+        <v>921321104054</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>1</v>
@@ -2960,10 +2967,10 @@
         <v>55</v>
       </c>
       <c r="C56" s="8">
-        <v>921321104050</v>
+        <v>921321104055</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E56" s="7" t="s">
         <v>1</v>
@@ -2991,10 +2998,10 @@
         <v>56</v>
       </c>
       <c r="C57" s="8">
-        <v>921321104051</v>
+        <v>921321104056</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>1</v>
@@ -3022,10 +3029,10 @@
         <v>57</v>
       </c>
       <c r="C58" s="8">
-        <v>921321104052</v>
+        <v>921321104057</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>1</v>
@@ -3053,10 +3060,10 @@
         <v>58</v>
       </c>
       <c r="C59" s="8">
-        <v>921321104053</v>
+        <v>921321104058</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>1</v>
@@ -3084,10 +3091,10 @@
         <v>59</v>
       </c>
       <c r="C60" s="8">
-        <v>921321104054</v>
+        <v>921321104059</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>1</v>
@@ -3115,10 +3122,10 @@
         <v>60</v>
       </c>
       <c r="C61" s="8">
-        <v>921321104055</v>
+        <v>921321104060</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>1</v>
@@ -3146,10 +3153,10 @@
         <v>61</v>
       </c>
       <c r="C62" s="8">
-        <v>921321104056</v>
+        <v>921321104061</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>1</v>
@@ -3177,10 +3184,10 @@
         <v>62</v>
       </c>
       <c r="C63" s="8">
-        <v>921321104057</v>
+        <v>921321104063</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>1</v>
@@ -3207,13 +3214,13 @@
       <c r="B64" s="5">
         <v>63</v>
       </c>
-      <c r="C64" s="8">
-        <v>921321104058</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E64" s="7" t="s">
+      <c r="C64" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F64" s="1"/>
@@ -3238,13 +3245,13 @@
       <c r="B65" s="5">
         <v>64</v>
       </c>
-      <c r="C65" s="8">
-        <v>921321104059</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E65" s="7" t="s">
+      <c r="C65" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F65" s="1"/>
@@ -3269,13 +3276,13 @@
       <c r="B66" s="5">
         <v>65</v>
       </c>
-      <c r="C66" s="8">
-        <v>921321104060</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E66" s="7" t="s">
+      <c r="C66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F66" s="1"/>
@@ -3300,13 +3307,13 @@
       <c r="B67" s="5">
         <v>66</v>
       </c>
-      <c r="C67" s="8">
-        <v>921321104061</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E67" s="7" t="s">
+      <c r="C67" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F67" s="1"/>
@@ -3331,13 +3338,13 @@
       <c r="B68" s="5">
         <v>67</v>
       </c>
-      <c r="C68" s="8">
-        <v>921321104063</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E68" s="7" t="s">
+      <c r="C68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F68" s="1"/>
@@ -3362,11 +3369,11 @@
       <c r="B69" s="5">
         <v>1</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>76</v>
+      <c r="C69" s="8">
+        <v>921321104062</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>74</v>
@@ -3393,11 +3400,11 @@
       <c r="B70" s="5">
         <v>2</v>
       </c>
-      <c r="C70" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>78</v>
+      <c r="C70" s="10">
+        <v>921321104064</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="E70" s="7" t="s">
         <v>74</v>
@@ -3424,11 +3431,11 @@
       <c r="B71" s="5">
         <v>3</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>80</v>
+      <c r="C71" s="8">
+        <v>921321104065</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>74</v>
@@ -3455,11 +3462,11 @@
       <c r="B72" s="5">
         <v>4</v>
       </c>
-      <c r="C72" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>82</v>
+      <c r="C72" s="8">
+        <v>921321104066</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>74</v>
@@ -3486,11 +3493,11 @@
       <c r="B73" s="5">
         <v>5</v>
       </c>
-      <c r="C73" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>84</v>
+      <c r="C73" s="8">
+        <v>921321104067</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>74</v>
@@ -3518,10 +3525,10 @@
         <v>6</v>
       </c>
       <c r="C74" s="8">
-        <v>921321104062</v>
+        <v>921321104068</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E74" s="7" t="s">
         <v>74</v>
@@ -3548,11 +3555,11 @@
       <c r="B75" s="5">
         <v>7</v>
       </c>
-      <c r="C75" s="10">
-        <v>921321104064</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>86</v>
+      <c r="C75" s="8">
+        <v>921321104069</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E75" s="7" t="s">
         <v>74</v>
@@ -3580,10 +3587,10 @@
         <v>8</v>
       </c>
       <c r="C76" s="8">
-        <v>921321104065</v>
+        <v>921321104070</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E76" s="7" t="s">
         <v>74</v>
@@ -3611,10 +3618,10 @@
         <v>9</v>
       </c>
       <c r="C77" s="8">
-        <v>921321104066</v>
+        <v>921321104071</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E77" s="7" t="s">
         <v>74</v>
@@ -3642,10 +3649,10 @@
         <v>10</v>
       </c>
       <c r="C78" s="8">
-        <v>921321104067</v>
+        <v>921321104072</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>74</v>
@@ -3673,10 +3680,10 @@
         <v>11</v>
       </c>
       <c r="C79" s="8">
-        <v>921321104068</v>
+        <v>921321104073</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>74</v>
@@ -3704,10 +3711,10 @@
         <v>12</v>
       </c>
       <c r="C80" s="8">
-        <v>921321104069</v>
+        <v>921321104074</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E80" s="7" t="s">
         <v>74</v>
@@ -3735,10 +3742,10 @@
         <v>13</v>
       </c>
       <c r="C81" s="8">
-        <v>921321104070</v>
+        <v>921321104075</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E81" s="7" t="s">
         <v>74</v>
@@ -3766,10 +3773,10 @@
         <v>14</v>
       </c>
       <c r="C82" s="8">
-        <v>921321104071</v>
+        <v>921321104076</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E82" s="7" t="s">
         <v>74</v>
@@ -3797,10 +3804,10 @@
         <v>15</v>
       </c>
       <c r="C83" s="8">
-        <v>921321104072</v>
+        <v>921321104077</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="E83" s="7" t="s">
         <v>74</v>
@@ -3827,11 +3834,11 @@
       <c r="B84" s="5">
         <v>16</v>
       </c>
-      <c r="C84" s="8">
-        <v>921321104073</v>
-      </c>
-      <c r="D84" s="9" t="s">
-        <v>95</v>
+      <c r="C84" s="10">
+        <v>921321104078</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="E84" s="7" t="s">
         <v>74</v>
@@ -3859,10 +3866,10 @@
         <v>17</v>
       </c>
       <c r="C85" s="8">
-        <v>921321104074</v>
+        <v>921321104079</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E85" s="7" t="s">
         <v>74</v>
@@ -3890,10 +3897,10 @@
         <v>18</v>
       </c>
       <c r="C86" s="8">
-        <v>921321104075</v>
+        <v>921321104080</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E86" s="7" t="s">
         <v>74</v>
@@ -3921,10 +3928,10 @@
         <v>19</v>
       </c>
       <c r="C87" s="8">
-        <v>921321104076</v>
+        <v>921321104081</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E87" s="7" t="s">
         <v>74</v>
@@ -3952,10 +3959,10 @@
         <v>20</v>
       </c>
       <c r="C88" s="8">
-        <v>921321104077</v>
+        <v>921321104082</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E88" s="7" t="s">
         <v>74</v>
@@ -3982,11 +3989,11 @@
       <c r="B89" s="5">
         <v>21</v>
       </c>
-      <c r="C89" s="10">
-        <v>921321104078</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>100</v>
+      <c r="C89" s="8">
+        <v>921321104083</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="E89" s="7" t="s">
         <v>74</v>
@@ -4014,10 +4021,10 @@
         <v>22</v>
       </c>
       <c r="C90" s="8">
-        <v>921321104079</v>
+        <v>921321104084</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E90" s="7" t="s">
         <v>74</v>
@@ -4045,10 +4052,10 @@
         <v>23</v>
       </c>
       <c r="C91" s="8">
-        <v>921321104080</v>
+        <v>921321104085</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>74</v>
@@ -4076,10 +4083,10 @@
         <v>24</v>
       </c>
       <c r="C92" s="8">
-        <v>921321104081</v>
+        <v>921321104086</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E92" s="7" t="s">
         <v>74</v>
@@ -4107,10 +4114,10 @@
         <v>25</v>
       </c>
       <c r="C93" s="8">
-        <v>921321104082</v>
+        <v>921321104087</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="E93" s="7" t="s">
         <v>74</v>
@@ -4138,10 +4145,10 @@
         <v>26</v>
       </c>
       <c r="C94" s="8">
-        <v>921321104083</v>
+        <v>921321104088</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E94" s="7" t="s">
         <v>74</v>
@@ -4169,10 +4176,10 @@
         <v>27</v>
       </c>
       <c r="C95" s="8">
-        <v>921321104084</v>
+        <v>921321104089</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>74</v>
@@ -4200,10 +4207,10 @@
         <v>28</v>
       </c>
       <c r="C96" s="8">
-        <v>921321104085</v>
+        <v>921321104090</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E96" s="7" t="s">
         <v>74</v>
@@ -4231,10 +4238,10 @@
         <v>29</v>
       </c>
       <c r="C97" s="8">
-        <v>921321104086</v>
+        <v>921321104091</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>74</v>
@@ -4262,10 +4269,10 @@
         <v>30</v>
       </c>
       <c r="C98" s="8">
-        <v>921321104087</v>
+        <v>921321104092</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>74</v>
@@ -4293,10 +4300,10 @@
         <v>31</v>
       </c>
       <c r="C99" s="8">
-        <v>921321104088</v>
+        <v>921321104093</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>74</v>
@@ -4323,11 +4330,11 @@
       <c r="B100" s="5">
         <v>32</v>
       </c>
-      <c r="C100" s="8">
-        <v>921321104089</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>111</v>
+      <c r="C100" s="10">
+        <v>921321104094</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="E100" s="7" t="s">
         <v>74</v>
@@ -4355,10 +4362,10 @@
         <v>33</v>
       </c>
       <c r="C101" s="8">
-        <v>921321104090</v>
+        <v>921321104096</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>74</v>
@@ -4386,10 +4393,10 @@
         <v>34</v>
       </c>
       <c r="C102" s="8">
-        <v>921321104091</v>
+        <v>921321104097</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>74</v>
@@ -4417,10 +4424,10 @@
         <v>35</v>
       </c>
       <c r="C103" s="8">
-        <v>921321104092</v>
+        <v>921321104098</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>74</v>
@@ -4448,10 +4455,10 @@
         <v>36</v>
       </c>
       <c r="C104" s="8">
-        <v>921321104093</v>
+        <v>921321104099</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>74</v>
@@ -4478,11 +4485,11 @@
       <c r="B105" s="5">
         <v>37</v>
       </c>
-      <c r="C105" s="10">
-        <v>921321104094</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>116</v>
+      <c r="C105" s="8">
+        <v>921321104100</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>74</v>
@@ -4510,10 +4517,10 @@
         <v>38</v>
       </c>
       <c r="C106" s="8">
-        <v>921321104096</v>
+        <v>921321104101</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>74</v>
@@ -4541,10 +4548,10 @@
         <v>39</v>
       </c>
       <c r="C107" s="8">
-        <v>921321104097</v>
+        <v>921321104102</v>
       </c>
       <c r="D107" s="9" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>74</v>
@@ -4572,10 +4579,10 @@
         <v>40</v>
       </c>
       <c r="C108" s="8">
-        <v>921321104098</v>
+        <v>921321104103</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>74</v>
@@ -4603,10 +4610,10 @@
         <v>41</v>
       </c>
       <c r="C109" s="8">
-        <v>921321104099</v>
+        <v>921321104104</v>
       </c>
       <c r="D109" s="9" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>74</v>
@@ -4634,10 +4641,10 @@
         <v>42</v>
       </c>
       <c r="C110" s="8">
-        <v>921321104100</v>
+        <v>921321104105</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>74</v>
@@ -4665,10 +4672,10 @@
         <v>43</v>
       </c>
       <c r="C111" s="8">
-        <v>921321104101</v>
+        <v>921321104106</v>
       </c>
       <c r="D111" s="9" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>74</v>
@@ -4696,10 +4703,10 @@
         <v>44</v>
       </c>
       <c r="C112" s="8">
-        <v>921321104102</v>
+        <v>921321104107</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E112" s="7" t="s">
         <v>74</v>
@@ -4727,10 +4734,10 @@
         <v>45</v>
       </c>
       <c r="C113" s="8">
-        <v>921321104103</v>
+        <v>921321104108</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>74</v>
@@ -4758,10 +4765,10 @@
         <v>46</v>
       </c>
       <c r="C114" s="8">
-        <v>921321104104</v>
+        <v>921321104109</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E114" s="7" t="s">
         <v>74</v>
@@ -4789,10 +4796,10 @@
         <v>47</v>
       </c>
       <c r="C115" s="8">
-        <v>921321104105</v>
+        <v>921321104110</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E115" s="7" t="s">
         <v>74</v>
@@ -4820,10 +4827,10 @@
         <v>48</v>
       </c>
       <c r="C116" s="8">
-        <v>921321104106</v>
+        <v>921321104111</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E116" s="7" t="s">
         <v>74</v>
@@ -4851,10 +4858,10 @@
         <v>49</v>
       </c>
       <c r="C117" s="8">
-        <v>921321104107</v>
+        <v>921321104112</v>
       </c>
       <c r="D117" s="9" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>74</v>
@@ -4882,10 +4889,10 @@
         <v>50</v>
       </c>
       <c r="C118" s="8">
-        <v>921321104108</v>
+        <v>921321104113</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E118" s="7" t="s">
         <v>74</v>
@@ -4913,10 +4920,10 @@
         <v>51</v>
       </c>
       <c r="C119" s="8">
-        <v>921321104109</v>
+        <v>921321104114</v>
       </c>
       <c r="D119" s="9" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E119" s="7" t="s">
         <v>74</v>
@@ -4944,10 +4951,10 @@
         <v>52</v>
       </c>
       <c r="C120" s="8">
-        <v>921321104110</v>
+        <v>921321104115</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E120" s="7" t="s">
         <v>74</v>
@@ -4975,10 +4982,10 @@
         <v>53</v>
       </c>
       <c r="C121" s="8">
-        <v>921321104111</v>
+        <v>921321104116</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E121" s="7" t="s">
         <v>74</v>
@@ -5006,10 +5013,10 @@
         <v>54</v>
       </c>
       <c r="C122" s="8">
-        <v>921321104112</v>
+        <v>921321104118</v>
       </c>
       <c r="D122" s="9" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>74</v>
@@ -5037,10 +5044,10 @@
         <v>55</v>
       </c>
       <c r="C123" s="8">
-        <v>921321104113</v>
+        <v>921321104119</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>74</v>
@@ -5068,10 +5075,10 @@
         <v>56</v>
       </c>
       <c r="C124" s="8">
-        <v>921321104114</v>
+        <v>921321104120</v>
       </c>
       <c r="D124" s="9" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>74</v>
@@ -5099,10 +5106,10 @@
         <v>57</v>
       </c>
       <c r="C125" s="8">
-        <v>921321104115</v>
+        <v>921321104121</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>74</v>
@@ -5130,10 +5137,10 @@
         <v>58</v>
       </c>
       <c r="C126" s="8">
-        <v>921321104116</v>
+        <v>921321104122</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>74</v>
@@ -5161,10 +5168,10 @@
         <v>59</v>
       </c>
       <c r="C127" s="8">
-        <v>921321104118</v>
+        <v>921321104123</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>74</v>
@@ -5192,10 +5199,10 @@
         <v>60</v>
       </c>
       <c r="C128" s="8">
-        <v>921321104119</v>
+        <v>921321104124</v>
       </c>
       <c r="D128" s="9" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E128" s="7" t="s">
         <v>74</v>
@@ -5223,10 +5230,10 @@
         <v>61</v>
       </c>
       <c r="C129" s="8">
-        <v>921321104120</v>
+        <v>921321104125</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>74</v>
@@ -5254,10 +5261,10 @@
         <v>62</v>
       </c>
       <c r="C130" s="8">
-        <v>921321104121</v>
+        <v>921321104126</v>
       </c>
       <c r="D130" s="9" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="E130" s="7" t="s">
         <v>74</v>
@@ -5284,11 +5291,11 @@
       <c r="B131" s="5">
         <v>63</v>
       </c>
-      <c r="C131" s="8">
-        <v>921321104122</v>
-      </c>
-      <c r="D131" s="9" t="s">
-        <v>142</v>
+      <c r="C131" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E131" s="7" t="s">
         <v>74</v>
@@ -5315,11 +5322,11 @@
       <c r="B132" s="5">
         <v>64</v>
       </c>
-      <c r="C132" s="8">
-        <v>921321104123</v>
-      </c>
-      <c r="D132" s="9" t="s">
-        <v>143</v>
+      <c r="C132" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E132" s="7" t="s">
         <v>74</v>
@@ -5346,11 +5353,11 @@
       <c r="B133" s="5">
         <v>65</v>
       </c>
-      <c r="C133" s="8">
-        <v>921321104124</v>
-      </c>
-      <c r="D133" s="9" t="s">
-        <v>144</v>
+      <c r="C133" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="E133" s="7" t="s">
         <v>74</v>
@@ -5377,11 +5384,11 @@
       <c r="B134" s="5">
         <v>66</v>
       </c>
-      <c r="C134" s="8">
-        <v>921321104125</v>
-      </c>
-      <c r="D134" s="9" t="s">
-        <v>145</v>
+      <c r="C134" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E134" s="7" t="s">
         <v>74</v>
@@ -5408,11 +5415,11 @@
       <c r="B135" s="5">
         <v>67</v>
       </c>
-      <c r="C135" s="8">
-        <v>921321104126</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>146</v>
+      <c r="C135" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="E135" s="7" t="s">
         <v>74</v>
@@ -5439,11 +5446,11 @@
       <c r="B136" s="5">
         <v>1</v>
       </c>
-      <c r="C136" s="5">
-        <v>92132113307</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>148</v>
+      <c r="C136" s="8">
+        <v>921321104127</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>147</v>
@@ -5470,11 +5477,11 @@
       <c r="B137" s="5">
         <v>2</v>
       </c>
-      <c r="C137" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>150</v>
+      <c r="C137" s="8">
+        <v>921321104128</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="E137" s="7" t="s">
         <v>147</v>
@@ -5501,11 +5508,11 @@
       <c r="B138" s="5">
         <v>3</v>
       </c>
-      <c r="C138" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>152</v>
+      <c r="C138" s="8">
+        <v>921321104129</v>
+      </c>
+      <c r="D138" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="E138" s="7" t="s">
         <v>147</v>
@@ -5532,11 +5539,11 @@
       <c r="B139" s="5">
         <v>4</v>
       </c>
-      <c r="C139" s="8">
-        <v>921321104127</v>
-      </c>
-      <c r="D139" s="9" t="s">
-        <v>153</v>
+      <c r="C139" s="10">
+        <v>921321104130</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>156</v>
       </c>
       <c r="E139" s="7" t="s">
         <v>147</v>
@@ -5564,10 +5571,10 @@
         <v>5</v>
       </c>
       <c r="C140" s="8">
-        <v>921321104128</v>
+        <v>921321104131</v>
       </c>
       <c r="D140" s="9" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E140" s="7" t="s">
         <v>147</v>
@@ -5595,10 +5602,10 @@
         <v>6</v>
       </c>
       <c r="C141" s="8">
-        <v>921321104129</v>
+        <v>921321104132</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E141" s="7" t="s">
         <v>147</v>
@@ -5625,11 +5632,11 @@
       <c r="B142" s="5">
         <v>7</v>
       </c>
-      <c r="C142" s="10">
-        <v>921321104130</v>
-      </c>
-      <c r="D142" s="7" t="s">
-        <v>156</v>
+      <c r="C142" s="8">
+        <v>921321104133</v>
+      </c>
+      <c r="D142" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="E142" s="7" t="s">
         <v>147</v>
@@ -5657,10 +5664,10 @@
         <v>8</v>
       </c>
       <c r="C143" s="8">
-        <v>921321104131</v>
+        <v>921321104134</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E143" s="7" t="s">
         <v>147</v>
@@ -5688,10 +5695,10 @@
         <v>9</v>
       </c>
       <c r="C144" s="8">
-        <v>921321104132</v>
+        <v>921321104135</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E144" s="7" t="s">
         <v>147</v>
@@ -5719,10 +5726,10 @@
         <v>10</v>
       </c>
       <c r="C145" s="8">
-        <v>921321104133</v>
+        <v>921321104136</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E145" s="7" t="s">
         <v>147</v>
@@ -5750,10 +5757,10 @@
         <v>11</v>
       </c>
       <c r="C146" s="8">
-        <v>921321104134</v>
+        <v>921321104137</v>
       </c>
       <c r="D146" s="9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E146" s="7" t="s">
         <v>147</v>
@@ -5781,10 +5788,10 @@
         <v>12</v>
       </c>
       <c r="C147" s="8">
-        <v>921321104135</v>
+        <v>921321104138</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="E147" s="7" t="s">
         <v>147</v>
@@ -5812,10 +5819,10 @@
         <v>13</v>
       </c>
       <c r="C148" s="8">
-        <v>921321104136</v>
+        <v>921321104139</v>
       </c>
       <c r="D148" s="9" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E148" s="7" t="s">
         <v>147</v>
@@ -5843,10 +5850,10 @@
         <v>14</v>
       </c>
       <c r="C149" s="8">
-        <v>921321104137</v>
+        <v>921321104140</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E149" s="7" t="s">
         <v>147</v>
@@ -5874,10 +5881,10 @@
         <v>15</v>
       </c>
       <c r="C150" s="8">
-        <v>921321104138</v>
+        <v>921321104141</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E150" s="7" t="s">
         <v>147</v>
@@ -5905,10 +5912,10 @@
         <v>16</v>
       </c>
       <c r="C151" s="8">
-        <v>921321104139</v>
+        <v>921321104142</v>
       </c>
       <c r="D151" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E151" s="7" t="s">
         <v>147</v>
@@ -5936,10 +5943,10 @@
         <v>17</v>
       </c>
       <c r="C152" s="8">
-        <v>921321104140</v>
+        <v>921321104143</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E152" s="7" t="s">
         <v>147</v>
@@ -5967,10 +5974,10 @@
         <v>18</v>
       </c>
       <c r="C153" s="8">
-        <v>921321104141</v>
+        <v>921321104144</v>
       </c>
       <c r="D153" s="9" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E153" s="7" t="s">
         <v>147</v>
@@ -5998,10 +6005,10 @@
         <v>19</v>
       </c>
       <c r="C154" s="8">
-        <v>921321104142</v>
+        <v>921321104145</v>
       </c>
       <c r="D154" s="9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E154" s="7" t="s">
         <v>147</v>
@@ -6029,10 +6036,10 @@
         <v>20</v>
       </c>
       <c r="C155" s="8">
-        <v>921321104143</v>
+        <v>921321104146</v>
       </c>
       <c r="D155" s="9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E155" s="7" t="s">
         <v>147</v>
@@ -6060,10 +6067,10 @@
         <v>21</v>
       </c>
       <c r="C156" s="8">
-        <v>921321104144</v>
+        <v>921321104147</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E156" s="7" t="s">
         <v>147</v>
@@ -6091,10 +6098,10 @@
         <v>22</v>
       </c>
       <c r="C157" s="8">
-        <v>921321104145</v>
+        <v>921321104148</v>
       </c>
       <c r="D157" s="9" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E157" s="7" t="s">
         <v>147</v>
@@ -6122,10 +6129,10 @@
         <v>23</v>
       </c>
       <c r="C158" s="8">
-        <v>921321104146</v>
+        <v>921321104150</v>
       </c>
       <c r="D158" s="9" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E158" s="7" t="s">
         <v>147</v>
@@ -6153,10 +6160,10 @@
         <v>24</v>
       </c>
       <c r="C159" s="8">
-        <v>921321104147</v>
+        <v>921321104151</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E159" s="7" t="s">
         <v>147</v>
@@ -6184,10 +6191,10 @@
         <v>25</v>
       </c>
       <c r="C160" s="8">
-        <v>921321104148</v>
+        <v>921321104152</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E160" s="7" t="s">
         <v>147</v>
@@ -6215,10 +6222,10 @@
         <v>26</v>
       </c>
       <c r="C161" s="8">
-        <v>921321104150</v>
+        <v>921321104153</v>
       </c>
       <c r="D161" s="9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E161" s="7" t="s">
         <v>147</v>
@@ -6246,10 +6253,10 @@
         <v>27</v>
       </c>
       <c r="C162" s="8">
-        <v>921321104151</v>
+        <v>921321104154</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E162" s="7" t="s">
         <v>147</v>
@@ -6277,10 +6284,10 @@
         <v>28</v>
       </c>
       <c r="C163" s="8">
-        <v>921321104152</v>
+        <v>921321104155</v>
       </c>
       <c r="D163" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E163" s="7" t="s">
         <v>147</v>
@@ -6308,10 +6315,10 @@
         <v>29</v>
       </c>
       <c r="C164" s="8">
-        <v>921321104153</v>
+        <v>921321104156</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="E164" s="7" t="s">
         <v>147</v>
@@ -6339,10 +6346,10 @@
         <v>30</v>
       </c>
       <c r="C165" s="8">
-        <v>921321104154</v>
+        <v>921321104157</v>
       </c>
       <c r="D165" s="9" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E165" s="7" t="s">
         <v>147</v>
@@ -6370,10 +6377,10 @@
         <v>31</v>
       </c>
       <c r="C166" s="8">
-        <v>921321104155</v>
+        <v>921321104158</v>
       </c>
       <c r="D166" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="E166" s="7" t="s">
         <v>147</v>
@@ -6401,10 +6408,10 @@
         <v>32</v>
       </c>
       <c r="C167" s="8">
-        <v>921321104156</v>
+        <v>921321104159</v>
       </c>
       <c r="D167" s="9" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E167" s="7" t="s">
         <v>147</v>
@@ -6432,10 +6439,10 @@
         <v>33</v>
       </c>
       <c r="C168" s="8">
-        <v>921321104157</v>
+        <v>921321104160</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E168" s="7" t="s">
         <v>147</v>
@@ -6463,10 +6470,10 @@
         <v>34</v>
       </c>
       <c r="C169" s="8">
-        <v>921321104158</v>
+        <v>921321104161</v>
       </c>
       <c r="D169" s="9" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E169" s="7" t="s">
         <v>147</v>
@@ -6494,10 +6501,10 @@
         <v>35</v>
       </c>
       <c r="C170" s="8">
-        <v>921321104159</v>
+        <v>921321104162</v>
       </c>
       <c r="D170" s="9" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="E170" s="7" t="s">
         <v>147</v>
@@ -6525,10 +6532,10 @@
         <v>36</v>
       </c>
       <c r="C171" s="8">
-        <v>921321104160</v>
+        <v>921321104163</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E171" s="7" t="s">
         <v>147</v>
@@ -6556,10 +6563,10 @@
         <v>37</v>
       </c>
       <c r="C172" s="8">
-        <v>921321104161</v>
+        <v>921321104164</v>
       </c>
       <c r="D172" s="9" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E172" s="7" t="s">
         <v>147</v>
@@ -6587,10 +6594,10 @@
         <v>38</v>
       </c>
       <c r="C173" s="8">
-        <v>921321104162</v>
+        <v>921321104165</v>
       </c>
       <c r="D173" s="9" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E173" s="7" t="s">
         <v>147</v>
@@ -6618,10 +6625,10 @@
         <v>39</v>
       </c>
       <c r="C174" s="8">
-        <v>921321104163</v>
+        <v>921321104166</v>
       </c>
       <c r="D174" s="9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E174" s="7" t="s">
         <v>147</v>
@@ -6649,10 +6656,10 @@
         <v>40</v>
       </c>
       <c r="C175" s="8">
-        <v>921321104164</v>
+        <v>921321104167</v>
       </c>
       <c r="D175" s="9" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E175" s="7" t="s">
         <v>147</v>
@@ -6680,10 +6687,10 @@
         <v>41</v>
       </c>
       <c r="C176" s="8">
-        <v>921321104165</v>
+        <v>921321104168</v>
       </c>
       <c r="D176" s="9" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E176" s="7" t="s">
         <v>147</v>
@@ -6711,10 +6718,10 @@
         <v>42</v>
       </c>
       <c r="C177" s="8">
-        <v>921321104166</v>
+        <v>921321104169</v>
       </c>
       <c r="D177" s="9" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E177" s="7" t="s">
         <v>147</v>
@@ -6742,10 +6749,10 @@
         <v>43</v>
       </c>
       <c r="C178" s="8">
-        <v>921321104167</v>
+        <v>921321104170</v>
       </c>
       <c r="D178" s="9" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E178" s="7" t="s">
         <v>147</v>
@@ -6773,10 +6780,10 @@
         <v>44</v>
       </c>
       <c r="C179" s="8">
-        <v>921321104168</v>
+        <v>921321104172</v>
       </c>
       <c r="D179" s="9" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E179" s="7" t="s">
         <v>147</v>
@@ -6804,10 +6811,10 @@
         <v>45</v>
       </c>
       <c r="C180" s="8">
-        <v>921321104169</v>
+        <v>921321104173</v>
       </c>
       <c r="D180" s="9" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E180" s="7" t="s">
         <v>147</v>
@@ -6835,10 +6842,10 @@
         <v>46</v>
       </c>
       <c r="C181" s="8">
-        <v>921321104170</v>
+        <v>921321104174</v>
       </c>
       <c r="D181" s="9" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E181" s="7" t="s">
         <v>147</v>
@@ -6866,10 +6873,10 @@
         <v>47</v>
       </c>
       <c r="C182" s="8">
-        <v>921321104172</v>
+        <v>921321104175</v>
       </c>
       <c r="D182" s="9" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E182" s="7" t="s">
         <v>147</v>
@@ -6897,10 +6904,10 @@
         <v>48</v>
       </c>
       <c r="C183" s="8">
-        <v>921321104173</v>
+        <v>921321104176</v>
       </c>
       <c r="D183" s="9" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E183" s="7" t="s">
         <v>147</v>
@@ -6928,10 +6935,10 @@
         <v>49</v>
       </c>
       <c r="C184" s="8">
-        <v>921321104174</v>
+        <v>921321104177</v>
       </c>
       <c r="D184" s="9" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="E184" s="7" t="s">
         <v>147</v>
@@ -6959,10 +6966,10 @@
         <v>50</v>
       </c>
       <c r="C185" s="8">
-        <v>921321104175</v>
+        <v>921321104178</v>
       </c>
       <c r="D185" s="9" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E185" s="7" t="s">
         <v>147</v>
@@ -6990,10 +6997,10 @@
         <v>51</v>
       </c>
       <c r="C186" s="8">
-        <v>921321104176</v>
+        <v>921321104179</v>
       </c>
       <c r="D186" s="9" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E186" s="7" t="s">
         <v>147</v>
@@ -7021,10 +7028,10 @@
         <v>52</v>
       </c>
       <c r="C187" s="8">
-        <v>921321104177</v>
+        <v>921321104180</v>
       </c>
       <c r="D187" s="9" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E187" s="7" t="s">
         <v>147</v>
@@ -7052,10 +7059,10 @@
         <v>53</v>
       </c>
       <c r="C188" s="8">
-        <v>921321104178</v>
+        <v>921321104181</v>
       </c>
       <c r="D188" s="9" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="E188" s="7" t="s">
         <v>147</v>
@@ -7083,10 +7090,10 @@
         <v>54</v>
       </c>
       <c r="C189" s="8">
-        <v>921321104179</v>
+        <v>921321104182</v>
       </c>
       <c r="D189" s="9" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E189" s="7" t="s">
         <v>147</v>
@@ -7114,10 +7121,10 @@
         <v>55</v>
       </c>
       <c r="C190" s="8">
-        <v>921321104180</v>
+        <v>921321104183</v>
       </c>
       <c r="D190" s="9" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="E190" s="7" t="s">
         <v>147</v>
@@ -7145,10 +7152,10 @@
         <v>56</v>
       </c>
       <c r="C191" s="8">
-        <v>921321104181</v>
+        <v>921321104184</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E191" s="7" t="s">
         <v>147</v>
@@ -7176,10 +7183,10 @@
         <v>57</v>
       </c>
       <c r="C192" s="8">
-        <v>921321104182</v>
+        <v>921321104185</v>
       </c>
       <c r="D192" s="9" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="E192" s="7" t="s">
         <v>147</v>
@@ -7207,10 +7214,10 @@
         <v>58</v>
       </c>
       <c r="C193" s="8">
-        <v>921321104183</v>
+        <v>921321104186</v>
       </c>
       <c r="D193" s="9" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E193" s="7" t="s">
         <v>147</v>
@@ -7238,10 +7245,10 @@
         <v>59</v>
       </c>
       <c r="C194" s="8">
-        <v>921321104184</v>
+        <v>921321104187</v>
       </c>
       <c r="D194" s="9" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="E194" s="7" t="s">
         <v>147</v>
@@ -7269,10 +7276,10 @@
         <v>60</v>
       </c>
       <c r="C195" s="8">
-        <v>921321104185</v>
+        <v>921321104188</v>
       </c>
       <c r="D195" s="9" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E195" s="7" t="s">
         <v>147</v>
@@ -7300,10 +7307,10 @@
         <v>61</v>
       </c>
       <c r="C196" s="8">
-        <v>921321104186</v>
+        <v>921321104190</v>
       </c>
       <c r="D196" s="9" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="E196" s="7" t="s">
         <v>147</v>
@@ -7331,10 +7338,10 @@
         <v>62</v>
       </c>
       <c r="C197" s="8">
-        <v>921321104187</v>
+        <v>921321104191</v>
       </c>
       <c r="D197" s="9" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E197" s="7" t="s">
         <v>147</v>
@@ -7361,11 +7368,11 @@
       <c r="B198" s="5">
         <v>63</v>
       </c>
-      <c r="C198" s="8">
-        <v>921321104188</v>
-      </c>
-      <c r="D198" s="9" t="s">
-        <v>212</v>
+      <c r="C198" s="5">
+        <v>92132113307</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="E198" s="7" t="s">
         <v>147</v>
@@ -7392,11 +7399,11 @@
       <c r="B199" s="5">
         <v>64</v>
       </c>
-      <c r="C199" s="8">
-        <v>921321104190</v>
-      </c>
-      <c r="D199" s="9" t="s">
-        <v>213</v>
+      <c r="C199" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="E199" s="7" t="s">
         <v>147</v>
@@ -7423,11 +7430,11 @@
       <c r="B200" s="5">
         <v>65</v>
       </c>
-      <c r="C200" s="8">
-        <v>921321104191</v>
-      </c>
-      <c r="D200" s="9" t="s">
-        <v>214</v>
+      <c r="C200" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="E200" s="7" t="s">
         <v>147</v>
@@ -7452,16 +7459,16 @@
         <v>200</v>
       </c>
       <c r="B201" s="5">
-        <v>1</v>
-      </c>
-      <c r="C201" s="5" t="s">
-        <v>216</v>
+        <v>66</v>
+      </c>
+      <c r="C201" s="5">
+        <v>9213211</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>217</v>
+        <v>292</v>
       </c>
       <c r="E201" s="7" t="s">
-        <v>215</v>
+        <v>147</v>
       </c>
       <c r="F201" s="1"/>
       <c r="G201" s="1"/>
@@ -7483,13 +7490,13 @@
         <v>201</v>
       </c>
       <c r="B202" s="5">
-        <v>2</v>
-      </c>
-      <c r="C202" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>219</v>
+        <v>1</v>
+      </c>
+      <c r="C202" s="8">
+        <v>921321104189</v>
+      </c>
+      <c r="D202" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="E202" s="7" t="s">
         <v>215</v>
@@ -7514,13 +7521,13 @@
         <v>202</v>
       </c>
       <c r="B203" s="5">
-        <v>3</v>
-      </c>
-      <c r="C203" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>221</v>
+        <v>2</v>
+      </c>
+      <c r="C203" s="8">
+        <v>921321104192</v>
+      </c>
+      <c r="D203" s="9" t="s">
+        <v>227</v>
       </c>
       <c r="E203" s="7" t="s">
         <v>215</v>
@@ -7545,13 +7552,13 @@
         <v>203</v>
       </c>
       <c r="B204" s="5">
-        <v>4</v>
-      </c>
-      <c r="C204" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>223</v>
+        <v>3</v>
+      </c>
+      <c r="C204" s="8">
+        <v>921321104193</v>
+      </c>
+      <c r="D204" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="E204" s="7" t="s">
         <v>215</v>
@@ -7576,13 +7583,13 @@
         <v>204</v>
       </c>
       <c r="B205" s="5">
-        <v>5</v>
-      </c>
-      <c r="C205" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>225</v>
+        <v>4</v>
+      </c>
+      <c r="C205" s="8">
+        <v>921321104194</v>
+      </c>
+      <c r="D205" s="9" t="s">
+        <v>229</v>
       </c>
       <c r="E205" s="7" t="s">
         <v>215</v>
@@ -7607,13 +7614,13 @@
         <v>205</v>
       </c>
       <c r="B206" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C206" s="8">
-        <v>921321104189</v>
+        <v>921321104195</v>
       </c>
       <c r="D206" s="9" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E206" s="7" t="s">
         <v>215</v>
@@ -7638,13 +7645,13 @@
         <v>206</v>
       </c>
       <c r="B207" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C207" s="8">
-        <v>921321104192</v>
+        <v>921321104196</v>
       </c>
       <c r="D207" s="9" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E207" s="7" t="s">
         <v>215</v>
@@ -7669,13 +7676,13 @@
         <v>207</v>
       </c>
       <c r="B208" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C208" s="8">
-        <v>921321104193</v>
+        <v>921321104197</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E208" s="7" t="s">
         <v>215</v>
@@ -7700,13 +7707,13 @@
         <v>208</v>
       </c>
       <c r="B209" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C209" s="8">
-        <v>921321104194</v>
+        <v>921321104198</v>
       </c>
       <c r="D209" s="9" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="E209" s="7" t="s">
         <v>215</v>
@@ -7731,13 +7738,13 @@
         <v>209</v>
       </c>
       <c r="B210" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C210" s="8">
-        <v>921321104195</v>
+        <v>921321104199</v>
       </c>
       <c r="D210" s="9" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E210" s="7" t="s">
         <v>215</v>
@@ -7762,13 +7769,13 @@
         <v>210</v>
       </c>
       <c r="B211" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C211" s="8">
-        <v>921321104196</v>
+        <v>921321104200</v>
       </c>
       <c r="D211" s="9" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E211" s="7" t="s">
         <v>215</v>
@@ -7793,13 +7800,13 @@
         <v>211</v>
       </c>
       <c r="B212" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C212" s="8">
-        <v>921321104197</v>
+        <v>921321104201</v>
       </c>
       <c r="D212" s="9" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E212" s="7" t="s">
         <v>215</v>
@@ -7824,13 +7831,13 @@
         <v>212</v>
       </c>
       <c r="B213" s="5">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C213" s="8">
-        <v>921321104198</v>
+        <v>921321104202</v>
       </c>
       <c r="D213" s="9" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="E213" s="7" t="s">
         <v>215</v>
@@ -7855,13 +7862,13 @@
         <v>213</v>
       </c>
       <c r="B214" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C214" s="8">
-        <v>921321104199</v>
+        <v>921321104203</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E214" s="7" t="s">
         <v>215</v>
@@ -7886,13 +7893,13 @@
         <v>214</v>
       </c>
       <c r="B215" s="5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C215" s="8">
-        <v>921321104200</v>
+        <v>921321104204</v>
       </c>
       <c r="D215" s="9" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E215" s="7" t="s">
         <v>215</v>
@@ -7917,13 +7924,13 @@
         <v>215</v>
       </c>
       <c r="B216" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C216" s="8">
-        <v>921321104201</v>
+        <v>921321104205</v>
       </c>
       <c r="D216" s="9" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E216" s="7" t="s">
         <v>215</v>
@@ -7948,13 +7955,13 @@
         <v>216</v>
       </c>
       <c r="B217" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C217" s="8">
-        <v>921321104202</v>
+        <v>921321104206</v>
       </c>
       <c r="D217" s="9" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="E217" s="7" t="s">
         <v>215</v>
@@ -7979,13 +7986,13 @@
         <v>217</v>
       </c>
       <c r="B218" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C218" s="8">
-        <v>921321104203</v>
+        <v>921321104207</v>
       </c>
       <c r="D218" s="9" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E218" s="7" t="s">
         <v>215</v>
@@ -8010,13 +8017,13 @@
         <v>218</v>
       </c>
       <c r="B219" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C219" s="8">
-        <v>921321104204</v>
+        <v>921321104208</v>
       </c>
       <c r="D219" s="9" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E219" s="7" t="s">
         <v>215</v>
@@ -8041,13 +8048,13 @@
         <v>219</v>
       </c>
       <c r="B220" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C220" s="8">
-        <v>921321104205</v>
+        <v>921321104209</v>
       </c>
       <c r="D220" s="9" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="E220" s="7" t="s">
         <v>215</v>
@@ -8072,13 +8079,13 @@
         <v>220</v>
       </c>
       <c r="B221" s="5">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C221" s="8">
-        <v>921321104206</v>
+        <v>921321104210</v>
       </c>
       <c r="D221" s="9" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E221" s="7" t="s">
         <v>215</v>
@@ -8103,13 +8110,13 @@
         <v>221</v>
       </c>
       <c r="B222" s="5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C222" s="8">
-        <v>921321104207</v>
+        <v>921321104211</v>
       </c>
       <c r="D222" s="9" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="E222" s="7" t="s">
         <v>215</v>
@@ -8134,13 +8141,13 @@
         <v>222</v>
       </c>
       <c r="B223" s="5">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C223" s="8">
-        <v>921321104208</v>
+        <v>921321104212</v>
       </c>
       <c r="D223" s="9" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="E223" s="7" t="s">
         <v>215</v>
@@ -8165,13 +8172,13 @@
         <v>223</v>
       </c>
       <c r="B224" s="5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C224" s="8">
-        <v>921321104209</v>
+        <v>921321104213</v>
       </c>
       <c r="D224" s="9" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E224" s="7" t="s">
         <v>215</v>
@@ -8196,13 +8203,13 @@
         <v>224</v>
       </c>
       <c r="B225" s="5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C225" s="8">
-        <v>921321104210</v>
+        <v>921321104214</v>
       </c>
       <c r="D225" s="9" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E225" s="7" t="s">
         <v>215</v>
@@ -8227,13 +8234,13 @@
         <v>225</v>
       </c>
       <c r="B226" s="5">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C226" s="8">
-        <v>921321104211</v>
+        <v>921321104215</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="E226" s="7" t="s">
         <v>215</v>
@@ -8258,13 +8265,13 @@
         <v>226</v>
       </c>
       <c r="B227" s="5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C227" s="8">
-        <v>921321104212</v>
+        <v>921321104216</v>
       </c>
       <c r="D227" s="9" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E227" s="7" t="s">
         <v>215</v>
@@ -8289,13 +8296,13 @@
         <v>227</v>
       </c>
       <c r="B228" s="5">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C228" s="8">
-        <v>921321104213</v>
+        <v>921321104217</v>
       </c>
       <c r="D228" s="9" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="E228" s="7" t="s">
         <v>215</v>
@@ -8320,13 +8327,13 @@
         <v>228</v>
       </c>
       <c r="B229" s="5">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C229" s="8">
-        <v>921321104214</v>
+        <v>921321104218</v>
       </c>
       <c r="D229" s="9" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E229" s="7" t="s">
         <v>215</v>
@@ -8351,13 +8358,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="5">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C230" s="8">
-        <v>921321104215</v>
+        <v>921321104219</v>
       </c>
       <c r="D230" s="9" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E230" s="7" t="s">
         <v>215</v>
@@ -8382,13 +8389,13 @@
         <v>230</v>
       </c>
       <c r="B231" s="5">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C231" s="8">
-        <v>921321104216</v>
+        <v>921321104220</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="E231" s="7" t="s">
         <v>215</v>
@@ -8413,13 +8420,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="5">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C232" s="8">
-        <v>921321104217</v>
+        <v>921321104221</v>
       </c>
       <c r="D232" s="9" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E232" s="7" t="s">
         <v>215</v>
@@ -8444,13 +8451,13 @@
         <v>232</v>
       </c>
       <c r="B233" s="5">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C233" s="8">
-        <v>921321104218</v>
+        <v>921321104222</v>
       </c>
       <c r="D233" s="9" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="E233" s="7" t="s">
         <v>215</v>
@@ -8475,13 +8482,13 @@
         <v>233</v>
       </c>
       <c r="B234" s="5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C234" s="8">
-        <v>921321104219</v>
+        <v>921321104223</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E234" s="7" t="s">
         <v>215</v>
@@ -8506,13 +8513,13 @@
         <v>234</v>
       </c>
       <c r="B235" s="5">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C235" s="8">
-        <v>921321104220</v>
+        <v>921321104224</v>
       </c>
       <c r="D235" s="9" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="E235" s="7" t="s">
         <v>215</v>
@@ -8537,13 +8544,13 @@
         <v>235</v>
       </c>
       <c r="B236" s="5">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C236" s="8">
-        <v>921321104221</v>
+        <v>921321104225</v>
       </c>
       <c r="D236" s="9" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="E236" s="7" t="s">
         <v>215</v>
@@ -8568,13 +8575,13 @@
         <v>236</v>
       </c>
       <c r="B237" s="5">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C237" s="8">
-        <v>921321104222</v>
+        <v>921321104226</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="E237" s="7" t="s">
         <v>215</v>
@@ -8599,13 +8606,13 @@
         <v>237</v>
       </c>
       <c r="B238" s="5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C238" s="8">
-        <v>921321104223</v>
+        <v>921321104227</v>
       </c>
       <c r="D238" s="9" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="E238" s="7" t="s">
         <v>215</v>
@@ -8630,13 +8637,13 @@
         <v>238</v>
       </c>
       <c r="B239" s="5">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C239" s="8">
-        <v>921321104224</v>
+        <v>921321104228</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="E239" s="7" t="s">
         <v>215</v>
@@ -8661,13 +8668,13 @@
         <v>239</v>
       </c>
       <c r="B240" s="5">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C240" s="8">
-        <v>921321104225</v>
+        <v>921321104229</v>
       </c>
       <c r="D240" s="9" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="E240" s="7" t="s">
         <v>215</v>
@@ -8692,13 +8699,13 @@
         <v>240</v>
       </c>
       <c r="B241" s="5">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C241" s="8">
-        <v>921321104226</v>
+        <v>921321104230</v>
       </c>
       <c r="D241" s="9" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="E241" s="7" t="s">
         <v>215</v>
@@ -8723,13 +8730,13 @@
         <v>241</v>
       </c>
       <c r="B242" s="5">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C242" s="8">
-        <v>921321104227</v>
+        <v>921321104231</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="E242" s="7" t="s">
         <v>215</v>
@@ -8754,13 +8761,13 @@
         <v>242</v>
       </c>
       <c r="B243" s="5">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C243" s="8">
-        <v>921321104228</v>
+        <v>921321104232</v>
       </c>
       <c r="D243" s="9" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="E243" s="7" t="s">
         <v>215</v>
@@ -8785,13 +8792,13 @@
         <v>243</v>
       </c>
       <c r="B244" s="5">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C244" s="8">
-        <v>921321104229</v>
+        <v>921321104233</v>
       </c>
       <c r="D244" s="9" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="E244" s="7" t="s">
         <v>215</v>
@@ -8816,13 +8823,13 @@
         <v>244</v>
       </c>
       <c r="B245" s="5">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C245" s="8">
-        <v>921321104230</v>
+        <v>921321104234</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E245" s="7" t="s">
         <v>215</v>
@@ -8847,13 +8854,13 @@
         <v>245</v>
       </c>
       <c r="B246" s="5">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C246" s="8">
-        <v>921321104231</v>
+        <v>921321104235</v>
       </c>
       <c r="D246" s="9" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="E246" s="7" t="s">
         <v>215</v>
@@ -8878,13 +8885,13 @@
         <v>246</v>
       </c>
       <c r="B247" s="5">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C247" s="8">
-        <v>921321104232</v>
+        <v>921321104236</v>
       </c>
       <c r="D247" s="9" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="E247" s="7" t="s">
         <v>215</v>
@@ -8909,13 +8916,13 @@
         <v>247</v>
       </c>
       <c r="B248" s="5">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C248" s="8">
-        <v>921321104233</v>
+        <v>921321104237</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E248" s="7" t="s">
         <v>215</v>
@@ -8940,13 +8947,13 @@
         <v>248</v>
       </c>
       <c r="B249" s="5">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C249" s="8">
-        <v>921321104234</v>
+        <v>921321104238</v>
       </c>
       <c r="D249" s="9" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="E249" s="7" t="s">
         <v>215</v>
@@ -8971,13 +8978,13 @@
         <v>249</v>
       </c>
       <c r="B250" s="5">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C250" s="8">
-        <v>921321104235</v>
+        <v>921321104239</v>
       </c>
       <c r="D250" s="9" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="E250" s="7" t="s">
         <v>215</v>
@@ -9002,13 +9009,13 @@
         <v>250</v>
       </c>
       <c r="B251" s="5">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C251" s="8">
-        <v>921321104236</v>
+        <v>921321104240</v>
       </c>
       <c r="D251" s="9" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E251" s="7" t="s">
         <v>215</v>
@@ -9033,13 +9040,13 @@
         <v>251</v>
       </c>
       <c r="B252" s="5">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C252" s="8">
-        <v>921321104237</v>
+        <v>921321104241</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E252" s="7" t="s">
         <v>215</v>
@@ -9064,13 +9071,13 @@
         <v>252</v>
       </c>
       <c r="B253" s="5">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C253" s="8">
-        <v>921321104238</v>
+        <v>921321104242</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="E253" s="7" t="s">
         <v>215</v>
@@ -9095,13 +9102,13 @@
         <v>253</v>
       </c>
       <c r="B254" s="5">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C254" s="8">
-        <v>921321104239</v>
+        <v>921321104243</v>
       </c>
       <c r="D254" s="9" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="E254" s="7" t="s">
         <v>215</v>
@@ -9126,13 +9133,13 @@
         <v>254</v>
       </c>
       <c r="B255" s="5">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C255" s="8">
-        <v>921321104240</v>
+        <v>921321104244</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="E255" s="7" t="s">
         <v>215</v>
@@ -9157,13 +9164,13 @@
         <v>255</v>
       </c>
       <c r="B256" s="5">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C256" s="8">
-        <v>921321104241</v>
+        <v>921321104245</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="E256" s="7" t="s">
         <v>215</v>
@@ -9188,13 +9195,13 @@
         <v>256</v>
       </c>
       <c r="B257" s="5">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C257" s="8">
-        <v>921321104242</v>
+        <v>921321104246</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="E257" s="7" t="s">
         <v>215</v>
@@ -9219,13 +9226,13 @@
         <v>257</v>
       </c>
       <c r="B258" s="5">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C258" s="8">
-        <v>921321104243</v>
+        <v>921321104247</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="E258" s="7" t="s">
         <v>215</v>
@@ -9250,13 +9257,13 @@
         <v>258</v>
       </c>
       <c r="B259" s="5">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C259" s="8">
-        <v>921321104244</v>
+        <v>921321104248</v>
       </c>
       <c r="D259" s="9" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="E259" s="7" t="s">
         <v>215</v>
@@ -9281,13 +9288,13 @@
         <v>259</v>
       </c>
       <c r="B260" s="5">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C260" s="8">
-        <v>921321104245</v>
+        <v>921321104249</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E260" s="7" t="s">
         <v>215</v>
@@ -9312,13 +9319,13 @@
         <v>260</v>
       </c>
       <c r="B261" s="5">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C261" s="8">
-        <v>921321104246</v>
+        <v>921321104250</v>
       </c>
       <c r="D261" s="9" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="E261" s="7" t="s">
         <v>215</v>
@@ -9343,13 +9350,13 @@
         <v>261</v>
       </c>
       <c r="B262" s="5">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C262" s="8">
-        <v>921321104247</v>
+        <v>921321104251</v>
       </c>
       <c r="D262" s="9" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E262" s="7" t="s">
         <v>215</v>
@@ -9374,13 +9381,13 @@
         <v>262</v>
       </c>
       <c r="B263" s="5">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C263" s="8">
-        <v>921321104248</v>
+        <v>921321104252</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E263" s="7" t="s">
         <v>215</v>
@@ -9405,13 +9412,13 @@
         <v>263</v>
       </c>
       <c r="B264" s="5">
-        <v>64</v>
-      </c>
-      <c r="C264" s="8">
-        <v>921321104249</v>
-      </c>
-      <c r="D264" s="9" t="s">
-        <v>284</v>
+        <v>63</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D264" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="E264" s="7" t="s">
         <v>215</v>
@@ -9436,13 +9443,13 @@
         <v>264</v>
       </c>
       <c r="B265" s="5">
-        <v>65</v>
-      </c>
-      <c r="C265" s="8">
-        <v>921321104250</v>
-      </c>
-      <c r="D265" s="9" t="s">
-        <v>285</v>
+        <v>64</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D265" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="E265" s="7" t="s">
         <v>215</v>
@@ -9467,13 +9474,13 @@
         <v>265</v>
       </c>
       <c r="B266" s="5">
-        <v>66</v>
-      </c>
-      <c r="C266" s="8">
-        <v>921321104251</v>
-      </c>
-      <c r="D266" s="9" t="s">
-        <v>286</v>
+        <v>65</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D266" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="E266" s="7" t="s">
         <v>215</v>
@@ -9498,13 +9505,13 @@
         <v>266</v>
       </c>
       <c r="B267" s="5">
-        <v>67</v>
-      </c>
-      <c r="C267" s="8">
-        <v>921321104252</v>
-      </c>
-      <c r="D267" s="9" t="s">
-        <v>287</v>
+        <v>66</v>
+      </c>
+      <c r="C267" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D267" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E267" s="7" t="s">
         <v>215</v>
@@ -9525,11 +9532,21 @@
       <c r="S267" s="1"/>
     </row>
     <row r="268" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="6"/>
-      <c r="B268" s="11"/>
-      <c r="C268" s="11"/>
-      <c r="D268" s="6"/>
-      <c r="E268" s="6"/>
+      <c r="A268" s="2">
+        <v>267</v>
+      </c>
+      <c r="B268" s="5">
+        <v>67</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D268" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E268" s="7" t="s">
+        <v>215</v>
+      </c>
       <c r="F268" s="1"/>
       <c r="G268" s="1"/>
       <c r="H268" s="1"/>
@@ -9546,11 +9563,21 @@
       <c r="S268" s="1"/>
     </row>
     <row r="269" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A269" s="6"/>
-      <c r="B269" s="11"/>
-      <c r="C269" s="11"/>
-      <c r="D269" s="6"/>
-      <c r="E269" s="6"/>
+      <c r="A269" s="2">
+        <v>268</v>
+      </c>
+      <c r="B269" s="11">
+        <v>68</v>
+      </c>
+      <c r="C269" s="11">
+        <v>9212110</v>
+      </c>
+      <c r="D269" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="E269" s="6" t="s">
+        <v>215</v>
+      </c>
       <c r="F269" s="1"/>
       <c r="G269" s="1"/>
       <c r="H269" s="1"/>
@@ -24790,90 +24817,6 @@
       <c r="Q994" s="1"/>
       <c r="R994" s="1"/>
       <c r="S994" s="1"/>
-    </row>
-    <row r="995" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A995" s="6"/>
-      <c r="B995" s="11"/>
-      <c r="C995" s="11"/>
-      <c r="D995" s="6"/>
-      <c r="E995" s="6"/>
-      <c r="F995" s="1"/>
-      <c r="G995" s="1"/>
-      <c r="H995" s="1"/>
-      <c r="I995" s="1"/>
-      <c r="J995" s="1"/>
-      <c r="K995" s="1"/>
-      <c r="L995" s="1"/>
-      <c r="M995" s="1"/>
-      <c r="N995" s="1"/>
-      <c r="O995" s="1"/>
-      <c r="P995" s="1"/>
-      <c r="Q995" s="1"/>
-      <c r="R995" s="1"/>
-      <c r="S995" s="1"/>
-    </row>
-    <row r="996" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A996" s="6"/>
-      <c r="B996" s="11"/>
-      <c r="C996" s="11"/>
-      <c r="D996" s="6"/>
-      <c r="E996" s="6"/>
-      <c r="F996" s="1"/>
-      <c r="G996" s="1"/>
-      <c r="H996" s="1"/>
-      <c r="I996" s="1"/>
-      <c r="J996" s="1"/>
-      <c r="K996" s="1"/>
-      <c r="L996" s="1"/>
-      <c r="M996" s="1"/>
-      <c r="N996" s="1"/>
-      <c r="O996" s="1"/>
-      <c r="P996" s="1"/>
-      <c r="Q996" s="1"/>
-      <c r="R996" s="1"/>
-      <c r="S996" s="1"/>
-    </row>
-    <row r="997" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A997" s="6"/>
-      <c r="B997" s="11"/>
-      <c r="C997" s="11"/>
-      <c r="D997" s="6"/>
-      <c r="E997" s="6"/>
-      <c r="F997" s="1"/>
-      <c r="G997" s="1"/>
-      <c r="H997" s="1"/>
-      <c r="I997" s="1"/>
-      <c r="J997" s="1"/>
-      <c r="K997" s="1"/>
-      <c r="L997" s="1"/>
-      <c r="M997" s="1"/>
-      <c r="N997" s="1"/>
-      <c r="O997" s="1"/>
-      <c r="P997" s="1"/>
-      <c r="Q997" s="1"/>
-      <c r="R997" s="1"/>
-      <c r="S997" s="1"/>
-    </row>
-    <row r="998" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A998" s="6"/>
-      <c r="B998" s="11"/>
-      <c r="C998" s="11"/>
-      <c r="D998" s="6"/>
-      <c r="E998" s="6"/>
-      <c r="F998" s="1"/>
-      <c r="G998" s="1"/>
-      <c r="H998" s="1"/>
-      <c r="I998" s="1"/>
-      <c r="J998" s="1"/>
-      <c r="K998" s="1"/>
-      <c r="L998" s="1"/>
-      <c r="M998" s="1"/>
-      <c r="N998" s="1"/>
-      <c r="O998" s="1"/>
-      <c r="P998" s="1"/>
-      <c r="Q998" s="1"/>
-      <c r="R998" s="1"/>
-      <c r="S998" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>